<commit_message>
Script Table 추가/ Object Table 캐릭터 ID생성/ Boss Table 시트 명 수정
Script Table 추가/ Object Table 캐릭터 ID생성/ Boss Table 시트 명 수정
</commit_message>
<xml_diff>
--- a/GameDesign/Table/TurtleBomb_Adventure_Boss_Table.xlsx
+++ b/GameDesign/Table/TurtleBomb_Adventure_Boss_Table.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" tabRatio="653"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12283" tabRatio="653"/>
   </bookViews>
   <sheets>
-    <sheet name="Table_Object" sheetId="8" r:id="rId1"/>
+    <sheet name="Table_Boss" sheetId="8" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -546,24 +546,24 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.600000000000001" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.35546875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" style="3" customWidth="1"/>
     <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26" customWidth="1"/>
-    <col min="9" max="9" width="23.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -595,7 +595,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
@@ -627,7 +627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -659,7 +659,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -693,7 +693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -727,7 +727,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -761,7 +761,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>4</v>
       </c>

</xml_diff>